<commit_message>
Update: Thêm tính năng gửi đơn multi-platform
</commit_message>
<xml_diff>
--- a/public/Template/TEMPLATE-MẪU.xlsx
+++ b/public/Template/TEMPLATE-MẪU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project Vue\TESTMENU\public\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA341377-821B-4F08-82EE-A3A11CD01FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4AEB76-87BF-4158-9C06-D01AC8B43CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-900" windowWidth="29040" windowHeight="15720" xr2:uid="{5674D665-1FCE-44F3-B15F-00AD865F5083}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5674D665-1FCE-44F3-B15F-00AD865F5083}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Ten_hang</t>
   </si>
@@ -67,13 +67,31 @@
   </si>
   <si>
     <t>Don_vi_tien_te</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>img_2</t>
+  </si>
+  <si>
+    <t>img_3</t>
+  </si>
+  <si>
+    <t>img_4</t>
+  </si>
+  <si>
+    <t>img_5</t>
+  </si>
+  <si>
+    <t>img_6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +132,14 @@
       <sz val="14"/>
       <color theme="0"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -170,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -210,6 +236,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -525,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A697A896-7A8E-47B8-982A-A63D4F819A7B}">
-  <dimension ref="A1:S52"/>
+  <dimension ref="A1:T52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +576,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
@@ -592,8 +619,26 @@
       <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
@@ -609,7 +654,7 @@
       <c r="M2" s="16"/>
       <c r="N2" s="13"/>
     </row>
-    <row r="3" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="14"/>
@@ -625,7 +670,7 @@
       <c r="M3" s="16"/>
       <c r="N3" s="13"/>
     </row>
-    <row r="4" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
       <c r="C4" s="14"/>
@@ -641,7 +686,7 @@
       <c r="M4" s="16"/>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="14"/>
@@ -657,7 +702,7 @@
       <c r="M5" s="16"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="14"/>
@@ -673,7 +718,7 @@
       <c r="M6" s="16"/>
       <c r="N6" s="13"/>
     </row>
-    <row r="7" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="14"/>
@@ -689,7 +734,7 @@
       <c r="M7" s="16"/>
       <c r="N7" s="13"/>
     </row>
-    <row r="8" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
@@ -705,7 +750,7 @@
       <c r="M8" s="16"/>
       <c r="N8" s="13"/>
     </row>
-    <row r="9" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="14"/>
@@ -721,7 +766,7 @@
       <c r="M9" s="16"/>
       <c r="N9" s="13"/>
     </row>
-    <row r="10" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14"/>
@@ -737,7 +782,7 @@
       <c r="M10" s="16"/>
       <c r="N10" s="13"/>
     </row>
-    <row r="11" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14"/>
@@ -753,7 +798,7 @@
       <c r="M11" s="16"/>
       <c r="N11" s="13"/>
     </row>
-    <row r="12" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
@@ -769,7 +814,7 @@
       <c r="M12" s="16"/>
       <c r="N12" s="13"/>
     </row>
-    <row r="13" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
@@ -785,7 +830,7 @@
       <c r="M13" s="16"/>
       <c r="N13" s="13"/>
     </row>
-    <row r="14" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
@@ -801,7 +846,7 @@
       <c r="M14" s="16"/>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="14"/>
@@ -817,7 +862,7 @@
       <c r="M15" s="16"/>
       <c r="N15" s="13"/>
     </row>
-    <row r="16" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="14"/>

</xml_diff>